<commit_message>
Commit boulot 12 février
</commit_message>
<xml_diff>
--- a/SonarLysaFX/Classeur1.xlsx
+++ b/SonarLysaFX/Classeur1.xlsx
@@ -1022,7 +1022,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,12 +1030,7 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
         <fgColor indexed="43"/>
       </patternFill>
     </fill>
@@ -1082,7 +1077,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3590">
+  <cellXfs count="2694">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1095,774 +1090,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="14" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -6471,774 +5698,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="8" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyFill="true" applyNumberFormat="1" borderId="0" fillId="9" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7543,7 +6002,7 @@
   <dimension ref="A1:O122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7646,86 +6105,86 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3142">
+      <c r="A3" s="2246">
         <v>1</v>
       </c>
-      <c r="B3" s="3143">
+      <c r="B3" s="2247">
         <v>254309</v>
       </c>
-      <c r="C3" s="3144" t="s">
+      <c r="C3" s="2248" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3145" t="s">
+      <c r="D3" s="2249" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3146" t="s">
+      <c r="E3" s="2250" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3147" t="s">
+      <c r="F3" s="2251" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3148">
+      <c r="G3" s="2252">
         <v>29</v>
       </c>
-      <c r="H3" s="3149">
+      <c r="H3" s="2253">
         <v>11</v>
       </c>
-      <c r="I3" s="3150">
+      <c r="I3" s="2254">
         <v>42871</v>
       </c>
-      <c r="J3" s="3151">
+      <c r="J3" s="2255">
         <v>42944</v>
       </c>
-      <c r="K3" s="3152"/>
-      <c r="L3" s="3153">
+      <c r="K3" s="2256"/>
+      <c r="L3" s="2257">
         <v>42871</v>
       </c>
-      <c r="M3" s="3154">
+      <c r="M3" s="2258">
         <v>43027</v>
       </c>
-      <c r="N3" s="3155">
+      <c r="N3" s="2259">
         <v>43043</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3156">
+      <c r="A4" s="2260">
         <v>2</v>
       </c>
-      <c r="B4" s="3157">
+      <c r="B4" s="2261">
         <v>259176</v>
       </c>
-      <c r="C4" s="3158" t="s">
+      <c r="C4" s="2262" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3159" t="s">
+      <c r="D4" s="2263" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3160" t="s">
+      <c r="E4" s="2264" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3161" t="s">
+      <c r="F4" s="2265" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3162">
+      <c r="G4" s="2266">
         <v>18</v>
       </c>
-      <c r="H4" s="3163">
+      <c r="H4" s="2267">
         <v>4</v>
       </c>
-      <c r="I4" s="3164">
+      <c r="I4" s="2268">
         <v>42934</v>
       </c>
-      <c r="J4" s="3165">
+      <c r="J4" s="2269">
         <v>43075</v>
       </c>
-      <c r="K4" s="3166"/>
-      <c r="L4" s="3167">
+      <c r="K4" s="2270"/>
+      <c r="L4" s="2271">
         <v>42934</v>
       </c>
-      <c r="M4" s="3168">
+      <c r="M4" s="2272">
         <v>43066</v>
       </c>
-      <c r="N4" s="3169">
+      <c r="N4" s="2273">
         <v>43085</v>
       </c>
     </row>
@@ -7769,86 +6228,86 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3170">
+      <c r="A6" s="2274">
         <v>4</v>
       </c>
-      <c r="B6" s="3171">
+      <c r="B6" s="2275">
         <v>265982</v>
       </c>
-      <c r="C6" s="3172" t="s">
+      <c r="C6" s="2276" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3173" t="s">
+      <c r="D6" s="2277" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3174" t="s">
+      <c r="E6" s="2278" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3175" t="s">
+      <c r="F6" s="2279" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="3176">
+      <c r="G6" s="2280">
         <v>31</v>
       </c>
-      <c r="H6" s="3177">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3178">
+      <c r="H6" s="2281">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2282">
         <v>42922</v>
       </c>
-      <c r="J6" s="3179">
+      <c r="J6" s="2283">
         <v>42927</v>
       </c>
-      <c r="K6" s="3180"/>
-      <c r="L6" s="3181">
+      <c r="K6" s="2284"/>
+      <c r="L6" s="2285">
         <v>42936</v>
       </c>
-      <c r="M6" s="3182">
+      <c r="M6" s="2286">
         <v>42968</v>
       </c>
-      <c r="N6" s="3183">
+      <c r="N6" s="2287">
         <v>43117</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3184">
+      <c r="A7" s="2288">
         <v>5</v>
       </c>
-      <c r="B7" s="3185">
+      <c r="B7" s="2289">
         <v>271174</v>
       </c>
-      <c r="C7" s="3186" t="s">
+      <c r="C7" s="2290" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3187" t="s">
+      <c r="D7" s="2291" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="3188" t="s">
+      <c r="E7" s="2292" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3189" t="s">
+      <c r="F7" s="2293" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3190">
+      <c r="G7" s="2294">
         <v>5</v>
       </c>
-      <c r="H7" s="3191">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3192">
+      <c r="H7" s="2295">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2296">
         <v>42962</v>
       </c>
-      <c r="J7" s="3193">
+      <c r="J7" s="2297">
         <v>42962</v>
       </c>
-      <c r="K7" s="3194"/>
-      <c r="L7" s="3195">
+      <c r="K7" s="2298"/>
+      <c r="L7" s="2299">
         <v>43073</v>
       </c>
-      <c r="M7" s="3196">
+      <c r="M7" s="2300">
         <v>43088</v>
       </c>
-      <c r="N7" s="3197">
+      <c r="N7" s="2301">
         <v>43112</v>
       </c>
     </row>
@@ -7886,44 +6345,44 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3198">
+      <c r="A9" s="2302">
         <v>7</v>
       </c>
-      <c r="B9" s="3199">
+      <c r="B9" s="2303">
         <v>276126</v>
       </c>
-      <c r="C9" s="3200" t="s">
+      <c r="C9" s="2304" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="3201" t="s">
+      <c r="D9" s="2305" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="3202" t="s">
+      <c r="E9" s="2306" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="3203" t="s">
+      <c r="F9" s="2307" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="3204">
+      <c r="G9" s="2308">
         <v>2</v>
       </c>
-      <c r="H9" s="3205">
+      <c r="H9" s="2309">
         <v>7</v>
       </c>
-      <c r="I9" s="3206">
+      <c r="I9" s="2310">
         <v>43038</v>
       </c>
-      <c r="J9" s="3207">
+      <c r="J9" s="2311">
         <v>43080</v>
       </c>
-      <c r="K9" s="3208"/>
-      <c r="L9" s="3209">
+      <c r="K9" s="2312"/>
+      <c r="L9" s="2313">
         <v>43038</v>
       </c>
-      <c r="M9" s="3210">
+      <c r="M9" s="2314">
         <v>43077</v>
       </c>
-      <c r="N9" s="3211">
+      <c r="N9" s="2315">
         <v>43126</v>
       </c>
     </row>
@@ -8000,44 +6459,44 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3212">
+      <c r="A12" s="2316">
         <v>10</v>
       </c>
-      <c r="B12" s="3213">
+      <c r="B12" s="2317">
         <v>282655</v>
       </c>
-      <c r="C12" s="3214" t="s">
+      <c r="C12" s="2318" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="3215" t="s">
+      <c r="D12" s="2319" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="3216" t="s">
+      <c r="E12" s="2320" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="3217" t="s">
+      <c r="F12" s="2321" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="3218">
+      <c r="G12" s="2322">
         <v>5</v>
       </c>
-      <c r="H12" s="3219">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3220">
+      <c r="H12" s="2323">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2324">
         <v>43017</v>
       </c>
-      <c r="J12" s="3221">
+      <c r="J12" s="2325">
         <v>43017</v>
       </c>
-      <c r="K12" s="3222"/>
-      <c r="L12" s="3223">
+      <c r="K12" s="2326"/>
+      <c r="L12" s="2327">
         <v>43048</v>
       </c>
-      <c r="M12" s="3224">
+      <c r="M12" s="2328">
         <v>43070</v>
       </c>
-      <c r="N12" s="3225">
+      <c r="N12" s="2329">
         <v>43108</v>
       </c>
     </row>
@@ -8120,128 +6579,128 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3226">
+      <c r="A15" s="2330">
         <v>13</v>
       </c>
-      <c r="B15" s="3227">
+      <c r="B15" s="2331">
         <v>283790</v>
       </c>
-      <c r="C15" s="3228" t="s">
+      <c r="C15" s="2332" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="3229" t="s">
+      <c r="D15" s="2333" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="3230" t="s">
+      <c r="E15" s="2334" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="3231" t="s">
+      <c r="F15" s="2335" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="3232">
+      <c r="G15" s="2336">
         <v>9</v>
       </c>
-      <c r="H15" s="3233">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3234">
+      <c r="H15" s="2337">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2338">
         <v>43025</v>
       </c>
-      <c r="J15" s="3235">
+      <c r="J15" s="2339">
         <v>43025</v>
       </c>
-      <c r="K15" s="3236"/>
-      <c r="L15" s="3237">
+      <c r="K15" s="2340"/>
+      <c r="L15" s="2341">
         <v>43027</v>
       </c>
-      <c r="M15" s="3238">
+      <c r="M15" s="2342">
         <v>43028</v>
       </c>
-      <c r="N15" s="3239">
+      <c r="N15" s="2343">
         <v>43103</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3240">
+      <c r="A16" s="2344">
         <v>14</v>
       </c>
-      <c r="B16" s="3241">
+      <c r="B16" s="2345">
         <v>283982</v>
       </c>
-      <c r="C16" s="3242" t="s">
+      <c r="C16" s="2346" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="3243" t="s">
+      <c r="D16" s="2347" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="3244" t="s">
+      <c r="E16" s="2348" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3245" t="s">
+      <c r="F16" s="2349" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="3246">
+      <c r="G16" s="2350">
         <v>7</v>
       </c>
-      <c r="H16" s="3247">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3248">
+      <c r="H16" s="2351">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2352">
         <v>43025</v>
       </c>
-      <c r="J16" s="3249">
+      <c r="J16" s="2353">
         <v>43025</v>
       </c>
-      <c r="K16" s="3250"/>
-      <c r="L16" s="3251">
+      <c r="K16" s="2354"/>
+      <c r="L16" s="2355">
         <v>43045</v>
       </c>
-      <c r="M16" s="3252">
+      <c r="M16" s="2356">
         <v>43088</v>
       </c>
-      <c r="N16" s="3253">
+      <c r="N16" s="2357">
         <v>43104</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="3254">
+      <c r="A17" s="2358">
         <v>15</v>
       </c>
-      <c r="B17" s="3255">
+      <c r="B17" s="2359">
         <v>284799</v>
       </c>
-      <c r="C17" s="3256" t="s">
+      <c r="C17" s="2360" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="3257" t="s">
+      <c r="D17" s="2361" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="3258" t="s">
+      <c r="E17" s="2362" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="3259" t="s">
+      <c r="F17" s="2363" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="3260">
+      <c r="G17" s="2364">
         <v>4</v>
       </c>
-      <c r="H17" s="3261">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3262">
+      <c r="H17" s="2365">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2366">
         <v>43033</v>
       </c>
-      <c r="J17" s="3263">
+      <c r="J17" s="2367">
         <v>43033</v>
       </c>
-      <c r="K17" s="3264"/>
-      <c r="L17" s="3265">
+      <c r="K17" s="2368"/>
+      <c r="L17" s="2369">
         <v>43111</v>
       </c>
-      <c r="M17" s="3266">
+      <c r="M17" s="2370">
         <v>43115</v>
       </c>
-      <c r="N17" s="3267">
+      <c r="N17" s="2371">
         <v>43125</v>
       </c>
     </row>
@@ -8402,44 +6861,44 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="3268">
+      <c r="A22" s="2372">
         <v>20</v>
       </c>
-      <c r="B22" s="3269">
+      <c r="B22" s="2373">
         <v>288870</v>
       </c>
-      <c r="C22" s="3270" t="s">
+      <c r="C22" s="2374" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="3271" t="s">
+      <c r="D22" s="2375" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="3272" t="s">
+      <c r="E22" s="2376" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="3273" t="s">
+      <c r="F22" s="2377" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="3274">
+      <c r="G22" s="2378">
         <v>3</v>
       </c>
-      <c r="H22" s="3275">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3276">
+      <c r="H22" s="2379">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2380">
         <v>43049</v>
       </c>
-      <c r="J22" s="3277">
+      <c r="J22" s="2381">
         <v>43052</v>
       </c>
-      <c r="K22" s="3278"/>
-      <c r="L22" s="3279">
+      <c r="K22" s="2382"/>
+      <c r="L22" s="2383">
         <v>43053</v>
       </c>
-      <c r="M22" s="3280">
+      <c r="M22" s="2384">
         <v>43069</v>
       </c>
-      <c r="N22" s="3281">
+      <c r="N22" s="2385">
         <v>43108</v>
       </c>
     </row>
@@ -8786,44 +7245,44 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="3282">
+      <c r="A32" s="2386">
         <v>30</v>
       </c>
-      <c r="B32" s="3283">
+      <c r="B32" s="2387">
         <v>292080</v>
       </c>
-      <c r="C32" s="3284" t="s">
+      <c r="C32" s="2388" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="3285" t="s">
+      <c r="D32" s="2389" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="3286" t="s">
+      <c r="E32" s="2390" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="3287" t="s">
+      <c r="F32" s="2391" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="3288">
+      <c r="G32" s="2392">
         <v>10</v>
       </c>
-      <c r="H32" s="3289">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3290">
+      <c r="H32" s="2393">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2394">
         <v>43066</v>
       </c>
-      <c r="J32" s="3291">
+      <c r="J32" s="2395">
         <v>43066</v>
       </c>
-      <c r="K32" s="3292"/>
-      <c r="L32" s="3293">
+      <c r="K32" s="2396"/>
+      <c r="L32" s="2397">
         <v>43070</v>
       </c>
-      <c r="M32" s="3294">
+      <c r="M32" s="2398">
         <v>43090</v>
       </c>
-      <c r="N32" s="3295">
+      <c r="N32" s="2399">
         <v>43117</v>
       </c>
     </row>
@@ -9089,86 +7548,86 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="3296">
+      <c r="A40" s="2400">
         <v>38</v>
       </c>
-      <c r="B40" s="3297">
+      <c r="B40" s="2401">
         <v>293720</v>
       </c>
-      <c r="C40" s="3298" t="s">
+      <c r="C40" s="2402" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="3299" t="s">
+      <c r="D40" s="2403" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="3300" t="s">
+      <c r="E40" s="2404" t="s">
         <v>140</v>
       </c>
-      <c r="F40" s="3301" t="s">
+      <c r="F40" s="2405" t="s">
         <v>141</v>
       </c>
-      <c r="G40" s="3302">
+      <c r="G40" s="2406">
         <v>6</v>
       </c>
-      <c r="H40" s="3303">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3304">
+      <c r="H40" s="2407">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2408">
         <v>43074</v>
       </c>
-      <c r="J40" s="3305">
+      <c r="J40" s="2409">
         <v>43074</v>
       </c>
-      <c r="K40" s="3306"/>
-      <c r="L40" s="3307">
+      <c r="K40" s="2410"/>
+      <c r="L40" s="2411">
         <v>43081</v>
       </c>
-      <c r="M40" s="3308">
+      <c r="M40" s="2412">
         <v>43115</v>
       </c>
-      <c r="N40" s="3309">
+      <c r="N40" s="2413">
         <v>43122</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="3310">
+      <c r="A41" s="2414">
         <v>39</v>
       </c>
-      <c r="B41" s="3311">
+      <c r="B41" s="2415">
         <v>293870</v>
       </c>
-      <c r="C41" s="3312" t="s">
+      <c r="C41" s="2416" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="3313" t="s">
+      <c r="D41" s="2417" t="s">
         <v>143</v>
       </c>
-      <c r="E41" s="3314" t="s">
+      <c r="E41" s="2418" t="s">
         <v>144</v>
       </c>
-      <c r="F41" s="3315" t="s">
+      <c r="F41" s="2419" t="s">
         <v>103</v>
       </c>
-      <c r="G41" s="3316">
+      <c r="G41" s="2420">
         <v>1</v>
       </c>
-      <c r="H41" s="3317">
-        <v>0</v>
-      </c>
-      <c r="I41" s="3318">
+      <c r="H41" s="2421">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2422">
         <v>43074</v>
       </c>
-      <c r="J41" s="3319">
+      <c r="J41" s="2423">
         <v>43074</v>
       </c>
-      <c r="K41" s="3320"/>
-      <c r="L41" s="3321">
+      <c r="K41" s="2424"/>
+      <c r="L41" s="2425">
         <v>43110</v>
       </c>
-      <c r="M41" s="3322">
+      <c r="M41" s="2426">
         <v>43112</v>
       </c>
-      <c r="N41" s="3323">
+      <c r="N41" s="2427">
         <v>43122</v>
       </c>
     </row>
@@ -9290,44 +7749,44 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="3324">
+      <c r="A45" s="2428">
         <v>43</v>
       </c>
-      <c r="B45" s="3325">
+      <c r="B45" s="2429">
         <v>294660</v>
       </c>
-      <c r="C45" s="3326" t="s">
+      <c r="C45" s="2430" t="s">
         <v>153</v>
       </c>
-      <c r="D45" s="3327" t="s">
+      <c r="D45" s="2431" t="s">
         <v>154</v>
       </c>
-      <c r="E45" s="3328" t="s">
+      <c r="E45" s="2432" t="s">
         <v>155</v>
       </c>
-      <c r="F45" s="3329" t="s">
+      <c r="F45" s="2433" t="s">
         <v>103</v>
       </c>
-      <c r="G45" s="3330">
+      <c r="G45" s="2434">
         <v>6</v>
       </c>
-      <c r="H45" s="3331">
+      <c r="H45" s="2435">
         <v>2</v>
       </c>
-      <c r="I45" s="3332">
+      <c r="I45" s="2436">
         <v>43090</v>
       </c>
-      <c r="J45" s="3333">
+      <c r="J45" s="2437">
         <v>43090</v>
       </c>
-      <c r="K45" s="3334"/>
-      <c r="L45" s="3335">
+      <c r="K45" s="2438"/>
+      <c r="L45" s="2439">
         <v>43090</v>
       </c>
-      <c r="M45" s="3336">
+      <c r="M45" s="2440">
         <v>43090</v>
       </c>
-      <c r="N45" s="3337">
+      <c r="N45" s="2441">
         <v>43117</v>
       </c>
     </row>
@@ -9605,44 +8064,44 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="3338">
+      <c r="A53" s="2442">
         <v>51</v>
       </c>
-      <c r="B53" s="3339">
+      <c r="B53" s="2443">
         <v>295424</v>
       </c>
-      <c r="C53" s="3340" t="s">
+      <c r="C53" s="2444" t="s">
         <v>167</v>
       </c>
-      <c r="D53" s="3341" t="s">
+      <c r="D53" s="2445" t="s">
         <v>168</v>
       </c>
-      <c r="E53" s="3342" t="s">
+      <c r="E53" s="2446" t="s">
         <v>169</v>
       </c>
-      <c r="F53" s="3343" t="s">
+      <c r="F53" s="2447" t="s">
         <v>103</v>
       </c>
-      <c r="G53" s="3344">
+      <c r="G53" s="2448">
         <v>1</v>
       </c>
-      <c r="H53" s="3345">
-        <v>0</v>
-      </c>
-      <c r="I53" s="3346">
+      <c r="H53" s="2449">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2450">
         <v>43082</v>
       </c>
-      <c r="J53" s="3347">
+      <c r="J53" s="2451">
         <v>43082</v>
       </c>
-      <c r="K53" s="3348"/>
-      <c r="L53" s="3349">
+      <c r="K53" s="2452"/>
+      <c r="L53" s="2453">
         <v>43105</v>
       </c>
-      <c r="M53" s="3350">
+      <c r="M53" s="2454">
         <v>43112</v>
       </c>
-      <c r="N53" s="3351">
+      <c r="N53" s="2455">
         <v>43116</v>
       </c>
     </row>
@@ -9686,128 +8145,128 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="3352">
+      <c r="A55" s="2456">
         <v>53</v>
       </c>
-      <c r="B55" s="3353">
+      <c r="B55" s="2457">
         <v>295493</v>
       </c>
-      <c r="C55" s="3354" t="s">
+      <c r="C55" s="2458" t="s">
         <v>172</v>
       </c>
-      <c r="D55" s="3355" t="s">
+      <c r="D55" s="2459" t="s">
         <v>173</v>
       </c>
-      <c r="E55" s="3356" t="s">
+      <c r="E55" s="2460" t="s">
         <v>174</v>
       </c>
-      <c r="F55" s="3357" t="s">
+      <c r="F55" s="2461" t="s">
         <v>175</v>
       </c>
-      <c r="G55" s="3358">
+      <c r="G55" s="2462">
         <v>1</v>
       </c>
-      <c r="H55" s="3359">
-        <v>0</v>
-      </c>
-      <c r="I55" s="3360">
+      <c r="H55" s="2463">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2464">
         <v>43082</v>
       </c>
-      <c r="J55" s="3361">
+      <c r="J55" s="2465">
         <v>43082</v>
       </c>
-      <c r="K55" s="3362"/>
-      <c r="L55" s="3363">
+      <c r="K55" s="2466"/>
+      <c r="L55" s="2467">
         <v>43096</v>
       </c>
-      <c r="M55" s="3364">
+      <c r="M55" s="2468">
         <v>43096</v>
       </c>
-      <c r="N55" s="3365">
+      <c r="N55" s="2469">
         <v>43112</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="3366">
+      <c r="A56" s="2470">
         <v>54</v>
       </c>
-      <c r="B56" s="3367">
+      <c r="B56" s="2471">
         <v>295507</v>
       </c>
-      <c r="C56" s="3368" t="s">
+      <c r="C56" s="2472" t="s">
         <v>176</v>
       </c>
-      <c r="D56" s="3369" t="s">
+      <c r="D56" s="2473" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="3370" t="s">
+      <c r="E56" s="2474" t="s">
         <v>178</v>
       </c>
-      <c r="F56" s="3371" t="s">
+      <c r="F56" s="2475" t="s">
         <v>35</v>
       </c>
-      <c r="G56" s="3372">
+      <c r="G56" s="2476">
         <v>1</v>
       </c>
-      <c r="H56" s="3373">
-        <v>0</v>
-      </c>
-      <c r="I56" s="3374">
+      <c r="H56" s="2477">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2478">
         <v>43082</v>
       </c>
-      <c r="J56" s="3375">
+      <c r="J56" s="2479">
         <v>43082</v>
       </c>
-      <c r="K56" s="3376"/>
-      <c r="L56" s="3377">
+      <c r="K56" s="2480"/>
+      <c r="L56" s="2481">
         <v>43090</v>
       </c>
-      <c r="M56" s="3378">
+      <c r="M56" s="2482">
         <v>43090</v>
       </c>
-      <c r="N56" s="3379">
+      <c r="N56" s="2483">
         <v>43112</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="3380">
+      <c r="A57" s="2484">
         <v>55</v>
       </c>
-      <c r="B57" s="3381">
+      <c r="B57" s="2485">
         <v>295529</v>
       </c>
-      <c r="C57" s="3382" t="s">
+      <c r="C57" s="2486" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="3383" t="s">
+      <c r="D57" s="2487" t="s">
         <v>180</v>
       </c>
-      <c r="E57" s="3384" t="s">
+      <c r="E57" s="2488" t="s">
         <v>181</v>
       </c>
-      <c r="F57" s="3385" t="s">
+      <c r="F57" s="2489" t="s">
         <v>35</v>
       </c>
-      <c r="G57" s="3386">
+      <c r="G57" s="2490">
         <v>1</v>
       </c>
-      <c r="H57" s="3387">
-        <v>0</v>
-      </c>
-      <c r="I57" s="3388">
+      <c r="H57" s="2491">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2492">
         <v>43084</v>
       </c>
-      <c r="J57" s="3389">
+      <c r="J57" s="2493">
         <v>43084</v>
       </c>
-      <c r="K57" s="3390"/>
-      <c r="L57" s="3391">
+      <c r="K57" s="2494"/>
+      <c r="L57" s="2495">
         <v>43084</v>
       </c>
-      <c r="M57" s="3392">
+      <c r="M57" s="2496">
         <v>43087</v>
       </c>
-      <c r="N57" s="3393">
+      <c r="N57" s="2497">
         <v>43112</v>
       </c>
     </row>
@@ -9851,44 +8310,44 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="3394">
+      <c r="A59" s="2498">
         <v>57</v>
       </c>
-      <c r="B59" s="3395">
+      <c r="B59" s="2499">
         <v>295683</v>
       </c>
-      <c r="C59" s="3396" t="s">
+      <c r="C59" s="2500" t="s">
         <v>185</v>
       </c>
-      <c r="D59" s="3397" t="s">
+      <c r="D59" s="2501" t="s">
         <v>101</v>
       </c>
-      <c r="E59" s="3398" t="s">
+      <c r="E59" s="2502" t="s">
         <v>186</v>
       </c>
-      <c r="F59" s="3399" t="s">
+      <c r="F59" s="2503" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="3400">
+      <c r="G59" s="2504">
         <v>2</v>
       </c>
-      <c r="H59" s="3401">
-        <v>0</v>
-      </c>
-      <c r="I59" s="3402">
+      <c r="H59" s="2505">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2506">
         <v>43083</v>
       </c>
-      <c r="J59" s="3403">
+      <c r="J59" s="2507">
         <v>43083</v>
       </c>
-      <c r="K59" s="3404"/>
-      <c r="L59" s="3405">
+      <c r="K59" s="2508"/>
+      <c r="L59" s="2509">
         <v>43083</v>
       </c>
-      <c r="M59" s="3406">
+      <c r="M59" s="2510">
         <v>43083</v>
       </c>
-      <c r="N59" s="3407">
+      <c r="N59" s="2511">
         <v>43122</v>
       </c>
     </row>
@@ -9929,44 +8388,44 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="3408">
+      <c r="A61" s="2512">
         <v>59</v>
       </c>
-      <c r="B61" s="3409">
+      <c r="B61" s="2513">
         <v>295880</v>
       </c>
-      <c r="C61" s="3410" t="s">
+      <c r="C61" s="2514" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="3411" t="s">
+      <c r="D61" s="2515" t="s">
         <v>191</v>
       </c>
-      <c r="E61" s="3412" t="s">
+      <c r="E61" s="2516" t="s">
         <v>88</v>
       </c>
-      <c r="F61" s="3413" t="s">
+      <c r="F61" s="2517" t="s">
         <v>103</v>
       </c>
-      <c r="G61" s="3414">
+      <c r="G61" s="2518">
         <v>6</v>
       </c>
-      <c r="H61" s="3415">
-        <v>0</v>
-      </c>
-      <c r="I61" s="3416">
+      <c r="H61" s="2519">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2520">
         <v>43084</v>
       </c>
-      <c r="J61" s="3417">
+      <c r="J61" s="2521">
         <v>43084</v>
       </c>
-      <c r="K61" s="3418"/>
-      <c r="L61" s="3419">
+      <c r="K61" s="2522"/>
+      <c r="L61" s="2523">
         <v>43084</v>
       </c>
-      <c r="M61" s="3420">
+      <c r="M61" s="2524">
         <v>43084</v>
       </c>
-      <c r="N61" s="3421">
+      <c r="N61" s="2525">
         <v>43119</v>
       </c>
     </row>
@@ -10088,44 +8547,44 @@
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="3422">
+      <c r="A65" s="2526">
         <v>63</v>
       </c>
-      <c r="B65" s="3423">
+      <c r="B65" s="2527">
         <v>296269</v>
       </c>
-      <c r="C65" s="3424" t="s">
+      <c r="C65" s="2528" t="s">
         <v>198</v>
       </c>
-      <c r="D65" s="3425" t="s">
+      <c r="D65" s="2529" t="s">
         <v>199</v>
       </c>
-      <c r="E65" s="3426" t="s">
+      <c r="E65" s="2530" t="s">
         <v>200</v>
       </c>
-      <c r="F65" s="3427" t="s">
+      <c r="F65" s="2531" t="s">
         <v>103</v>
       </c>
-      <c r="G65" s="3428">
+      <c r="G65" s="2532">
         <v>2</v>
       </c>
-      <c r="H65" s="3429">
-        <v>0</v>
-      </c>
-      <c r="I65" s="3430">
+      <c r="H65" s="2533">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2534">
         <v>43087</v>
       </c>
-      <c r="J65" s="3431">
+      <c r="J65" s="2535">
         <v>43087</v>
       </c>
-      <c r="K65" s="3432"/>
-      <c r="L65" s="3433">
+      <c r="K65" s="2536"/>
+      <c r="L65" s="2537">
         <v>43087</v>
       </c>
-      <c r="M65" s="3434">
+      <c r="M65" s="2538">
         <v>43105</v>
       </c>
-      <c r="N65" s="3435">
+      <c r="N65" s="2539">
         <v>43117</v>
       </c>
     </row>
@@ -10253,86 +8712,86 @@
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="3436">
+      <c r="A69" s="2540">
         <v>67</v>
       </c>
-      <c r="B69" s="3437">
+      <c r="B69" s="2541">
         <v>296973</v>
       </c>
-      <c r="C69" s="3438" t="s">
+      <c r="C69" s="2542" t="s">
         <v>211</v>
       </c>
-      <c r="D69" s="3439" t="s">
+      <c r="D69" s="2543" t="s">
         <v>212</v>
       </c>
-      <c r="E69" s="3440" t="s">
+      <c r="E69" s="2544" t="s">
         <v>213</v>
       </c>
-      <c r="F69" s="3441" t="s">
+      <c r="F69" s="2545" t="s">
         <v>103</v>
       </c>
-      <c r="G69" s="3442">
+      <c r="G69" s="2546">
         <v>1</v>
       </c>
-      <c r="H69" s="3443">
-        <v>0</v>
-      </c>
-      <c r="I69" s="3444">
+      <c r="H69" s="2547">
+        <v>0</v>
+      </c>
+      <c r="I69" s="2548">
         <v>43090</v>
       </c>
-      <c r="J69" s="3445">
+      <c r="J69" s="2549">
         <v>43091</v>
       </c>
-      <c r="K69" s="3446"/>
-      <c r="L69" s="3447">
+      <c r="K69" s="2550"/>
+      <c r="L69" s="2551">
         <v>43091</v>
       </c>
-      <c r="M69" s="3448">
+      <c r="M69" s="2552">
         <v>43091</v>
       </c>
-      <c r="N69" s="3449">
+      <c r="N69" s="2553">
         <v>43122</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="3450">
+      <c r="A70" s="2554">
         <v>68</v>
       </c>
-      <c r="B70" s="3451">
+      <c r="B70" s="2555">
         <v>297312</v>
       </c>
-      <c r="C70" s="3452" t="s">
+      <c r="C70" s="2556" t="s">
         <v>214</v>
       </c>
-      <c r="D70" s="3453" t="s">
+      <c r="D70" s="2557" t="s">
         <v>33</v>
       </c>
-      <c r="E70" s="3454" t="s">
+      <c r="E70" s="2558" t="s">
         <v>34</v>
       </c>
-      <c r="F70" s="3455" t="s">
+      <c r="F70" s="2559" t="s">
         <v>35</v>
       </c>
-      <c r="G70" s="3456">
+      <c r="G70" s="2560">
         <v>1</v>
       </c>
-      <c r="H70" s="3457">
-        <v>0</v>
-      </c>
-      <c r="I70" s="3458">
+      <c r="H70" s="2561">
+        <v>0</v>
+      </c>
+      <c r="I70" s="2562">
         <v>43090</v>
       </c>
-      <c r="J70" s="3459">
+      <c r="J70" s="2563">
         <v>43095</v>
       </c>
-      <c r="K70" s="3460"/>
-      <c r="L70" s="3461">
+      <c r="K70" s="2564"/>
+      <c r="L70" s="2565">
         <v>43109</v>
       </c>
-      <c r="M70" s="3462">
+      <c r="M70" s="2566">
         <v>43112</v>
       </c>
-      <c r="N70" s="3463">
+      <c r="N70" s="2567">
         <v>43112</v>
       </c>
     </row>
@@ -10448,44 +8907,44 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="3464">
+      <c r="A74" s="2568">
         <v>72</v>
       </c>
-      <c r="B74" s="3465">
+      <c r="B74" s="2569">
         <v>297547</v>
       </c>
-      <c r="C74" s="3466" t="s">
+      <c r="C74" s="2570" t="s">
         <v>222</v>
       </c>
-      <c r="D74" s="3467" t="s">
+      <c r="D74" s="2571" t="s">
         <v>223</v>
       </c>
-      <c r="E74" s="3468" t="s">
+      <c r="E74" s="2572" t="s">
         <v>224</v>
       </c>
-      <c r="F74" s="3469" t="s">
+      <c r="F74" s="2573" t="s">
         <v>103</v>
       </c>
-      <c r="G74" s="3470">
+      <c r="G74" s="2574">
         <v>3</v>
       </c>
-      <c r="H74" s="3471">
-        <v>0</v>
-      </c>
-      <c r="I74" s="3472">
+      <c r="H74" s="2575">
+        <v>0</v>
+      </c>
+      <c r="I74" s="2576">
         <v>43102</v>
       </c>
-      <c r="J74" s="3473">
+      <c r="J74" s="2577">
         <v>43102</v>
       </c>
-      <c r="K74" s="3474"/>
-      <c r="L74" s="3475">
+      <c r="K74" s="2578"/>
+      <c r="L74" s="2579">
         <v>43104</v>
       </c>
-      <c r="M74" s="3476">
+      <c r="M74" s="2580">
         <v>43112</v>
       </c>
-      <c r="N74" s="3477">
+      <c r="N74" s="2581">
         <v>43118</v>
       </c>
     </row>
@@ -10568,44 +9027,44 @@
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" s="3478">
+      <c r="A77" s="2582">
         <v>75</v>
       </c>
-      <c r="B77" s="3479">
+      <c r="B77" s="2583">
         <v>297695</v>
       </c>
-      <c r="C77" s="3480" t="s">
+      <c r="C77" s="2584" t="s">
         <v>229</v>
       </c>
-      <c r="D77" s="3481" t="s">
+      <c r="D77" s="2585" t="s">
         <v>230</v>
       </c>
-      <c r="E77" s="3482" t="s">
+      <c r="E77" s="2586" t="s">
         <v>231</v>
       </c>
-      <c r="F77" s="3483" t="s">
+      <c r="F77" s="2587" t="s">
         <v>103</v>
       </c>
-      <c r="G77" s="3484">
+      <c r="G77" s="2588">
         <v>1</v>
       </c>
-      <c r="H77" s="3485">
-        <v>0</v>
-      </c>
-      <c r="I77" s="3486">
+      <c r="H77" s="2589">
+        <v>0</v>
+      </c>
+      <c r="I77" s="2590">
         <v>43095</v>
       </c>
-      <c r="J77" s="3487">
+      <c r="J77" s="2591">
         <v>43095</v>
       </c>
-      <c r="K77" s="3488"/>
-      <c r="L77" s="3489">
+      <c r="K77" s="2592"/>
+      <c r="L77" s="2593">
         <v>43103</v>
       </c>
-      <c r="M77" s="3490">
+      <c r="M77" s="2594">
         <v>43111</v>
       </c>
-      <c r="N77" s="3491">
+      <c r="N77" s="2595">
         <v>43122</v>
       </c>
     </row>
@@ -10955,44 +9414,44 @@
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="3492">
+      <c r="A87" s="2596">
         <v>85</v>
       </c>
-      <c r="B87" s="3493">
+      <c r="B87" s="2597">
         <v>298688</v>
       </c>
-      <c r="C87" s="3494" t="s">
+      <c r="C87" s="2598" t="s">
         <v>253</v>
       </c>
-      <c r="D87" s="3495" t="s">
+      <c r="D87" s="2599" t="s">
         <v>254</v>
       </c>
-      <c r="E87" s="3496" t="s">
+      <c r="E87" s="2600" t="s">
         <v>255</v>
       </c>
-      <c r="F87" s="3497" t="s">
+      <c r="F87" s="2601" t="s">
         <v>103</v>
       </c>
-      <c r="G87" s="3498">
+      <c r="G87" s="2602">
         <v>2</v>
       </c>
-      <c r="H87" s="3499">
-        <v>0</v>
-      </c>
-      <c r="I87" s="3500">
+      <c r="H87" s="2603">
+        <v>0</v>
+      </c>
+      <c r="I87" s="2604">
         <v>43104</v>
       </c>
-      <c r="J87" s="3501">
+      <c r="J87" s="2605">
         <v>43104</v>
       </c>
-      <c r="K87" s="3502"/>
-      <c r="L87" s="3503">
+      <c r="K87" s="2606"/>
+      <c r="L87" s="2607">
         <v>43110</v>
       </c>
-      <c r="M87" s="3504">
+      <c r="M87" s="2608">
         <v>43110</v>
       </c>
-      <c r="N87" s="3505">
+      <c r="N87" s="2609">
         <v>43118</v>
       </c>
     </row>
@@ -11039,44 +9498,44 @@
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="3506">
+      <c r="A89" s="2610">
         <v>87</v>
       </c>
-      <c r="B89" s="3507">
+      <c r="B89" s="2611">
         <v>298823</v>
       </c>
-      <c r="C89" s="3508" t="s">
+      <c r="C89" s="2612" t="s">
         <v>258</v>
       </c>
-      <c r="D89" s="3509" t="s">
+      <c r="D89" s="2613" t="s">
         <v>259</v>
       </c>
-      <c r="E89" s="3510" t="s">
+      <c r="E89" s="2614" t="s">
         <v>260</v>
       </c>
-      <c r="F89" s="3511" t="s">
+      <c r="F89" s="2615" t="s">
         <v>103</v>
       </c>
-      <c r="G89" s="3512">
+      <c r="G89" s="2616">
         <v>6</v>
       </c>
-      <c r="H89" s="3513">
-        <v>0</v>
-      </c>
-      <c r="I89" s="3514">
+      <c r="H89" s="2617">
+        <v>0</v>
+      </c>
+      <c r="I89" s="2618">
         <v>43108</v>
       </c>
-      <c r="J89" s="3515">
+      <c r="J89" s="2619">
         <v>43108</v>
       </c>
-      <c r="K89" s="3516"/>
-      <c r="L89" s="3517">
+      <c r="K89" s="2620"/>
+      <c r="L89" s="2621">
         <v>43110</v>
       </c>
-      <c r="M89" s="3518">
+      <c r="M89" s="2622">
         <v>43111</v>
       </c>
-      <c r="N89" s="3519">
+      <c r="N89" s="2623">
         <v>43119</v>
       </c>
     </row>
@@ -11159,44 +9618,44 @@
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="3520">
+      <c r="A92" s="2624">
         <v>90</v>
       </c>
-      <c r="B92" s="3521">
+      <c r="B92" s="2625">
         <v>299137</v>
       </c>
-      <c r="C92" s="3522" t="s">
+      <c r="C92" s="2626" t="s">
         <v>265</v>
       </c>
-      <c r="D92" s="3523" t="s">
+      <c r="D92" s="2627" t="s">
         <v>139</v>
       </c>
-      <c r="E92" s="3524" t="s">
+      <c r="E92" s="2628" t="s">
         <v>140</v>
       </c>
-      <c r="F92" s="3525" t="s">
+      <c r="F92" s="2629" t="s">
         <v>266</v>
       </c>
-      <c r="G92" s="3526">
+      <c r="G92" s="2630">
         <v>7</v>
       </c>
-      <c r="H92" s="3527">
-        <v>0</v>
-      </c>
-      <c r="I92" s="3528">
+      <c r="H92" s="2631">
+        <v>0</v>
+      </c>
+      <c r="I92" s="2632">
         <v>43108</v>
       </c>
-      <c r="J92" s="3529">
+      <c r="J92" s="2633">
         <v>43108</v>
       </c>
-      <c r="K92" s="3530"/>
-      <c r="L92" s="3531">
+      <c r="K92" s="2634"/>
+      <c r="L92" s="2635">
         <v>43110</v>
       </c>
-      <c r="M92" s="3532">
+      <c r="M92" s="2636">
         <v>43117</v>
       </c>
-      <c r="N92" s="3533">
+      <c r="N92" s="2637">
         <v>43118</v>
       </c>
     </row>
@@ -11313,44 +9772,44 @@
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="3534">
+      <c r="A96" s="2638">
         <v>94</v>
       </c>
-      <c r="B96" s="3535">
+      <c r="B96" s="2639">
         <v>299669</v>
       </c>
-      <c r="C96" s="3536" t="s">
+      <c r="C96" s="2640" t="s">
         <v>275</v>
       </c>
-      <c r="D96" s="3537" t="s">
+      <c r="D96" s="2641" t="s">
         <v>276</v>
       </c>
-      <c r="E96" s="3538" t="s">
+      <c r="E96" s="2642" t="s">
         <v>277</v>
       </c>
-      <c r="F96" s="3539" t="s">
+      <c r="F96" s="2643" t="s">
         <v>103</v>
       </c>
-      <c r="G96" s="3540">
+      <c r="G96" s="2644">
         <v>1</v>
       </c>
-      <c r="H96" s="3541">
-        <v>0</v>
-      </c>
-      <c r="I96" s="3542">
+      <c r="H96" s="2645">
+        <v>0</v>
+      </c>
+      <c r="I96" s="2646">
         <v>43110</v>
       </c>
-      <c r="J96" s="3543">
+      <c r="J96" s="2647">
         <v>43110</v>
       </c>
-      <c r="K96" s="3544"/>
-      <c r="L96" s="3545">
+      <c r="K96" s="2648"/>
+      <c r="L96" s="2649">
         <v>43110</v>
       </c>
-      <c r="M96" s="3546">
+      <c r="M96" s="2650">
         <v>43122</v>
       </c>
-      <c r="N96" s="3547">
+      <c r="N96" s="2651">
         <v>43122</v>
       </c>
     </row>
@@ -11667,86 +10126,86 @@
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A105" s="3548">
+      <c r="A105" s="2652">
         <v>103</v>
       </c>
-      <c r="B105" s="3549">
+      <c r="B105" s="2653">
         <v>301543</v>
       </c>
-      <c r="C105" s="3550" t="s">
+      <c r="C105" s="2654" t="s">
         <v>294</v>
       </c>
-      <c r="D105" s="3551" t="s">
+      <c r="D105" s="2655" t="s">
         <v>295</v>
       </c>
-      <c r="E105" s="3552" t="s">
+      <c r="E105" s="2656" t="s">
         <v>296</v>
       </c>
-      <c r="F105" s="3553" t="s">
+      <c r="F105" s="2657" t="s">
         <v>297</v>
       </c>
-      <c r="G105" s="3554">
+      <c r="G105" s="2658">
         <v>6</v>
       </c>
-      <c r="H105" s="3555">
-        <v>0</v>
-      </c>
-      <c r="I105" s="3556">
+      <c r="H105" s="2659">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2660">
         <v>43119</v>
       </c>
-      <c r="J105" s="3557">
+      <c r="J105" s="2661">
         <v>43119</v>
       </c>
-      <c r="K105" s="3558"/>
-      <c r="L105" s="3559">
+      <c r="K105" s="2662"/>
+      <c r="L105" s="2663">
         <v>43119</v>
       </c>
-      <c r="M105" s="3560">
+      <c r="M105" s="2664">
         <v>43122</v>
       </c>
-      <c r="N105" s="3561">
+      <c r="N105" s="2665">
         <v>43125</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A106" s="3562">
+      <c r="A106" s="2666">
         <v>104</v>
       </c>
-      <c r="B106" s="3563">
+      <c r="B106" s="2667">
         <v>301604</v>
       </c>
-      <c r="C106" s="3564" t="s">
+      <c r="C106" s="2668" t="s">
         <v>298</v>
       </c>
-      <c r="D106" s="3565" t="s">
+      <c r="D106" s="2669" t="s">
         <v>299</v>
       </c>
-      <c r="E106" s="3566" t="s">
+      <c r="E106" s="2670" t="s">
         <v>178</v>
       </c>
-      <c r="F106" s="3567" t="s">
+      <c r="F106" s="2671" t="s">
         <v>297</v>
       </c>
-      <c r="G106" s="3568">
+      <c r="G106" s="2672">
         <v>7</v>
       </c>
-      <c r="H106" s="3569">
-        <v>0</v>
-      </c>
-      <c r="I106" s="3570">
+      <c r="H106" s="2673">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2674">
         <v>43119</v>
       </c>
-      <c r="J106" s="3571">
+      <c r="J106" s="2675">
         <v>43119</v>
       </c>
-      <c r="K106" s="3572"/>
-      <c r="L106" s="3573">
+      <c r="K106" s="2676"/>
+      <c r="L106" s="2677">
         <v>43123</v>
       </c>
-      <c r="M106" s="3574">
+      <c r="M106" s="2678">
         <v>43123</v>
       </c>
-      <c r="N106" s="3575">
+      <c r="N106" s="2679">
         <v>43130</v>
       </c>
     </row>
@@ -11937,44 +10396,44 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A112" s="3576">
+      <c r="A112" s="2680">
         <v>110</v>
       </c>
-      <c r="B112" s="3577">
+      <c r="B112" s="2681">
         <v>302315</v>
       </c>
-      <c r="C112" s="3578" t="s">
+      <c r="C112" s="2682" t="s">
         <v>313</v>
       </c>
-      <c r="D112" s="3579" t="s">
+      <c r="D112" s="2683" t="s">
         <v>33</v>
       </c>
-      <c r="E112" s="3580" t="s">
+      <c r="E112" s="2684" t="s">
         <v>279</v>
       </c>
-      <c r="F112" s="3581" t="s">
+      <c r="F112" s="2685" t="s">
         <v>297</v>
       </c>
-      <c r="G112" s="3582">
+      <c r="G112" s="2686">
         <v>7</v>
       </c>
-      <c r="H112" s="3583">
-        <v>0</v>
-      </c>
-      <c r="I112" s="3584">
+      <c r="H112" s="2687">
+        <v>0</v>
+      </c>
+      <c r="I112" s="2688">
         <v>43123</v>
       </c>
-      <c r="J112" s="3585">
+      <c r="J112" s="2689">
         <v>43123</v>
       </c>
-      <c r="K112" s="3586"/>
-      <c r="L112" s="3587">
+      <c r="K112" s="2690"/>
+      <c r="L112" s="2691">
         <v>43123</v>
       </c>
-      <c r="M112" s="3588">
+      <c r="M112" s="2692">
         <v>43123</v>
       </c>
-      <c r="N112" s="3589">
+      <c r="N112" s="2693">
         <v>43126</v>
       </c>
     </row>

</xml_diff>